<commit_message>
Update R script and FST files
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aki\Desktop\P.borealis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aki\Desktop\P.borealis\P.borealis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1022BB-9C1E-4969-BA8A-B3B321BAF8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5D3C7B-0E9B-4C44-9EB9-AEC9DCBB5145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="114">
   <si>
     <t>Tray-Grp1-10</t>
   </si>
@@ -386,8 +386,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -437,8 +437,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,17 +755,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FECA95-16D6-40EE-B346-590AE5A2B3B4}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="G86" sqref="G86:G91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +787,7 @@
         <v>10_SU18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +809,7 @@
         <v>11_SU18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -831,7 +831,7 @@
         <v>13_SU18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -853,7 +853,7 @@
         <v>17_SU18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -875,7 +875,7 @@
         <v>18_SU18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -897,7 +897,7 @@
         <v>19_SU18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -919,7 +919,7 @@
         <v>20_SU18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -941,7 +941,7 @@
         <v>21_SU18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -963,7 +963,7 @@
         <v>22_SU18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -985,7 +985,7 @@
         <v>23_SU18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>24_SU18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>3_SU18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>6_SU18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>7_SU18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>9_SU18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>26_AR18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>29_AR18</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>30_AR18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>31_AR18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>32_AR18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>33_AR18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>34_AR18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>36_AR18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>39_AR18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>41_AR18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>42_AR18</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>43_AR18</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>44_AR18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>45_AR18</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>47_AR18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>48_AR18</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>52_SI18</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>53_SI18</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>56_SI18</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>57_SI18</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>58_SI18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>59_SI18</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>60_SI18</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>66_SI18</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>67_SI18</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>68_SI18</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>70_SI18</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>71_SI18</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>72_SI18</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>74_SD18</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>75_SD18</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>76_SD18</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>78_SD18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>79_SD18</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>80_SD18</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>81_SD18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>84_SD18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>86_SD18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>87_SD18</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>88_SD18</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>89_SD18</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>90_SD18</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>91_SD18</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>92_SD18</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>94_SD18</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>1_YS21</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>10_YS21</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>11_YS21</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>12_YS21</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>2_YS21</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>3_YS21</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>4_YS21</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>5_YS21</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>6_YS21</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>7_YS21</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>8_YS21</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>9_YS21</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>66_IS21</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>67_IS21</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>68_IS21</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>69_IS21</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>70_IS21</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>71_IS21</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>72_IS21</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>73_IS21</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>74_IS21</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>75_IS21</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>76_IS21</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>141_UH21</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>142_UH21</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>143_UH21</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>144_UH21</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>145_UH21</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>146_UH21</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>147_UH21</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>148_UH21</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>149_UH21</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>150_UH21</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2891,27 +2891,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65617DA5-2132-4A76-A1E9-67144CD93F3D}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -2948,11 +2947,8 @@
       <c r="N1" t="s">
         <v>113</v>
       </c>
-      <c r="O1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2990,11 +2986,8 @@
       <c r="N2" s="5">
         <v>4.5215999999999999E-2</v>
       </c>
-      <c r="O2" s="5">
-        <v>4.5215999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3032,11 +3025,8 @@
       <c r="N3" s="5">
         <v>4.1324E-2</v>
       </c>
-      <c r="O3" s="5">
-        <v>4.1324E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3074,11 +3064,8 @@
       <c r="N4" s="5">
         <v>3.2585000000000003E-2</v>
       </c>
-      <c r="O4" s="5">
-        <v>3.2585000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -3116,11 +3103,8 @@
       <c r="N5" s="5">
         <v>2.1308000000000001E-2</v>
       </c>
-      <c r="O5" s="5">
-        <v>2.1308000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -3158,11 +3142,8 @@
       <c r="N6" s="5">
         <v>6.7832999999999999E-3</v>
       </c>
-      <c r="O6" s="5">
-        <v>6.7832999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -3200,11 +3181,8 @@
       <c r="N7" s="5">
         <v>5.8323999999999997E-3</v>
       </c>
-      <c r="O7" s="5">
-        <v>5.8323999999999997E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -3242,11 +3220,8 @@
       <c r="N8" s="5">
         <v>5.1181999999999998E-3</v>
       </c>
-      <c r="O8" s="5">
-        <v>5.1181999999999998E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -3284,11 +3259,8 @@
       <c r="N9" s="5">
         <v>4.5439E-3</v>
       </c>
-      <c r="O9" s="5">
-        <v>4.5439E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -3326,11 +3298,8 @@
       <c r="N10" s="5">
         <v>4.3807999999999998E-3</v>
       </c>
-      <c r="O10" s="5">
-        <v>4.3807999999999998E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -3355,11 +3324,8 @@
       <c r="N11" s="5">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="O11" s="5">
-        <v>4.2700000000000004E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -3384,11 +3350,8 @@
       <c r="N12" s="5">
         <v>3.2943E-3</v>
       </c>
-      <c r="O12" s="5">
-        <v>3.2943E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -3413,11 +3376,8 @@
       <c r="N13" s="5">
         <v>2.9826000000000001E-4</v>
       </c>
-      <c r="O13" s="5">
-        <v>2.9826000000000001E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -3431,7 +3391,7 @@
         <v>4.5439E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -3445,7 +3405,7 @@
         <v>4.3807999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -3459,7 +3419,7 @@
         <v>4.2700000000000004E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -3473,7 +3433,7 @@
         <v>4.0623999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -3487,7 +3447,7 @@
         <v>3.3005999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>107</v>
       </c>
@@ -3501,7 +3461,7 @@
         <v>3.2943E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -3515,7 +3475,7 @@
         <v>2.7491999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>108</v>
       </c>
@@ -3529,7 +3489,7 @@
         <v>9.2086999999999996E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Update R script and sample file
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aki\Desktop\P.borealis\P.borealis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CBA251-E620-4C47-B0AE-D6CB80929CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAF0D9C-7F8A-4168-BC61-68E0B224E52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="117">
   <si>
     <t>Tray-Grp1-10</t>
   </si>
@@ -379,6 +380,15 @@
   </si>
   <si>
     <t>WC_weighted_FST</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>Pop</t>
   </si>
 </sst>
 </file>
@@ -755,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FECA95-16D6-40EE-B346-590AE5A2B3B4}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G86" sqref="G86:G91"/>
     </sheetView>
   </sheetViews>
@@ -2893,7 +2903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65617DA5-2132-4A76-A1E9-67144CD93F3D}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3510,4 +3520,436 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B10706-462F-441C-8A3C-A38751A4306B}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="A11:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>0.106</v>
+      </c>
+      <c r="C5">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="D5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="E6">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.374</v>
+      </c>
+      <c r="G7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13">
+        <v>2.7492240000000002E-3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14">
+        <v>7.8321199999999997E-3</v>
+      </c>
+      <c r="C14">
+        <v>4.7663849999999997E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>3.3005629999999998E-3</v>
+      </c>
+      <c r="C15">
+        <v>4.0624279999999999E-3</v>
+      </c>
+      <c r="D15">
+        <v>5.9278723000000004E-3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16">
+        <v>5.832439E-3</v>
+      </c>
+      <c r="C16">
+        <v>4.2699840000000001E-3</v>
+      </c>
+      <c r="D16">
+        <v>2.9826160000000001E-4</v>
+      </c>
+      <c r="E16">
+        <v>3.2943080000000001E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17">
+        <v>6.783323E-3</v>
+      </c>
+      <c r="C17">
+        <v>5.118175E-3</v>
+      </c>
+      <c r="D17">
+        <v>4.5439466999999999E-3</v>
+      </c>
+      <c r="E17">
+        <v>4.3807760000000003E-3</v>
+      </c>
+      <c r="F17">
+        <v>9.208749E-4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18">
+        <v>4.5215666000000002E-2</v>
+      </c>
+      <c r="C18">
+        <v>3.2584531999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>2.1307997499999998E-2</v>
+      </c>
+      <c r="E18">
+        <v>4.1324086000000003E-2</v>
+      </c>
+      <c r="F18">
+        <v>1.33642404E-2</v>
+      </c>
+      <c r="G18">
+        <v>3.0229550000000001E-2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Sample sheet and images
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aki\Desktop\P.borealis\P.borealis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAF0D9C-7F8A-4168-BC61-68E0B224E52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8331D2-C84F-41DE-AD67-B3F51C9B96E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AE63C2DC-5148-4494-8A9B-D0F9B49C6674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="119">
   <si>
     <t>Tray-Grp1-10</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>Pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WC FST </t>
+  </si>
+  <si>
+    <t>p-value with 1000 bootstrap</t>
   </si>
 </sst>
 </file>
@@ -2903,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65617DA5-2132-4A76-A1E9-67144CD93F3D}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,6 +2923,7 @@
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3524,72 +3531,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B10706-462F-441C-8A3C-A38751A4306B}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="A11:H18"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3">
-        <v>0.13400000000000001</v>
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>114</v>
@@ -3612,13 +3598,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C4">
-        <v>4.9000000000000002E-2</v>
+        <v>2.7492240000000002E-3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
       </c>
       <c r="D4" t="s">
         <v>114</v>
@@ -3638,16 +3624,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5">
-        <v>0.106</v>
+        <v>7.8321199999999997E-3</v>
       </c>
       <c r="C5">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="D5">
-        <v>2.7E-2</v>
+        <v>4.7663849999999997E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
       </c>
       <c r="E5" t="s">
         <v>114</v>
@@ -3664,19 +3650,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6">
-        <v>1.0999999999999999E-2</v>
+        <v>3.3005629999999998E-3</v>
       </c>
       <c r="C6">
-        <v>2.9000000000000001E-2</v>
+        <v>4.0624279999999999E-3</v>
       </c>
       <c r="D6">
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="E6">
-        <v>0.10199999999999999</v>
+        <v>5.9278723000000004E-3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
       </c>
       <c r="F6" t="s">
         <v>114</v>
@@ -3690,22 +3676,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7">
-        <v>4.0000000000000001E-3</v>
+        <v>5.832439E-3</v>
       </c>
       <c r="C7">
-        <v>1.4999999999999999E-2</v>
+        <v>4.2699840000000001E-3</v>
       </c>
       <c r="D7">
-        <v>4.2000000000000003E-2</v>
+        <v>2.9826160000000001E-4</v>
       </c>
       <c r="E7">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.374</v>
+        <v>3.2943080000000001E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
       </c>
       <c r="G7" t="s">
         <v>114</v>
@@ -3716,88 +3702,93 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8">
+        <v>6.783323E-3</v>
+      </c>
+      <c r="C8">
+        <v>5.118175E-3</v>
+      </c>
+      <c r="D8">
+        <v>4.5439466999999999E-3</v>
+      </c>
+      <c r="E8">
+        <v>4.3807760000000003E-3</v>
+      </c>
+      <c r="F8">
+        <v>9.208749E-4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>109</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="B9">
+        <v>4.5215666000000002E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.2584531999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>2.1307997499999998E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.1324086000000003E-2</v>
+      </c>
+      <c r="F9">
+        <v>1.33642404E-2</v>
+      </c>
+      <c r="G9">
+        <v>3.0229550000000001E-2</v>
+      </c>
+      <c r="H9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
         <v>103</v>
       </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13">
-        <v>2.7492240000000002E-3</v>
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>114</v>
@@ -3820,13 +3811,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B14">
-        <v>7.8321199999999997E-3</v>
-      </c>
-      <c r="C14">
-        <v>4.7663849999999997E-3</v>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>114</v>
       </c>
       <c r="D14" t="s">
         <v>114</v>
@@ -3846,16 +3837,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B15">
-        <v>3.3005629999999998E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C15">
-        <v>4.0624279999999999E-3</v>
-      </c>
-      <c r="D15">
-        <v>5.9278723000000004E-3</v>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
       </c>
       <c r="E15" t="s">
         <v>114</v>
@@ -3872,19 +3863,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16">
-        <v>5.832439E-3</v>
+        <v>0.106</v>
       </c>
       <c r="C16">
-        <v>4.2699840000000001E-3</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="D16">
-        <v>2.9826160000000001E-4</v>
-      </c>
-      <c r="E16">
-        <v>3.2943080000000001E-3</v>
+        <v>2.7E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>114</v>
       </c>
       <c r="F16" t="s">
         <v>114</v>
@@ -3898,22 +3889,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17">
-        <v>6.783323E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C17">
-        <v>5.118175E-3</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D17">
-        <v>4.5439466999999999E-3</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="E17">
-        <v>4.3807760000000003E-3</v>
-      </c>
-      <c r="F17">
-        <v>9.208749E-4</v>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>114</v>
       </c>
       <c r="G17" t="s">
         <v>114</v>
@@ -3924,27 +3915,53 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E18">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.374</v>
+      </c>
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>109</v>
       </c>
-      <c r="B18">
-        <v>4.5215666000000002E-2</v>
-      </c>
-      <c r="C18">
-        <v>3.2584531999999999E-2</v>
-      </c>
-      <c r="D18">
-        <v>2.1307997499999998E-2</v>
-      </c>
-      <c r="E18">
-        <v>4.1324086000000003E-2</v>
-      </c>
-      <c r="F18">
-        <v>1.33642404E-2</v>
-      </c>
-      <c r="G18">
-        <v>3.0229550000000001E-2</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>